<commit_message>
working on importing data - currently routing of radar chart not working
</commit_message>
<xml_diff>
--- a/Minutes/April Minutes.xlsx
+++ b/Minutes/April Minutes.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51dcfef833b97180/Documents/Masters/Group Project/Minutes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessw\Documents\Group Project\desk23\Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{7BA893E6-832A-49FB-BDF3-6085246EE8C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4A7F2D3F-1743-4434-B571-3A572D635F5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE8D51A-955E-4082-9F13-CE3B15D561A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
+    <workbookView xWindow="1110" yWindow="300" windowWidth="14775" windowHeight="15300" activeTab="2" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
   </bookViews>
   <sheets>
     <sheet name="0604" sheetId="1" r:id="rId1"/>
     <sheet name="0704" sheetId="2" r:id="rId2"/>
+    <sheet name="0804" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
   <si>
     <t>Date:</t>
   </si>
@@ -143,13 +144,82 @@
   </si>
   <si>
     <t>Debug test site, connect our own data to the charts currently up</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Completed and debugged</t>
+  </si>
+  <si>
+    <t>Created colour blocked version</t>
+  </si>
+  <si>
+    <t>Hamza typescript crash course</t>
+  </si>
+  <si>
+    <t>On track</t>
+  </si>
+  <si>
+    <t>Stanni designing globe</t>
+  </si>
+  <si>
+    <t>Working on it</t>
+  </si>
+  <si>
+    <t>Wenda building server</t>
+  </si>
+  <si>
+    <t>Connect database to charts</t>
+  </si>
+  <si>
+    <t>Wenda and Jess</t>
+  </si>
+  <si>
+    <t>This week(end)</t>
+  </si>
+  <si>
+    <t>Get data from CSV file into database</t>
+  </si>
+  <si>
+    <t>Jess (with advice from Stanni)</t>
+  </si>
+  <si>
+    <t>Feedback sessions</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Prototype with fluorescent colours, darker ocean</t>
+  </si>
+  <si>
+    <t>Emily to help Wenda and Jess get back end off the ground if necessary</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=k5E2AVpwsko&amp;t=2086s&amp;ab_channel=ProgrammingwithMosh</t>
+  </si>
+  <si>
+    <t>https://docs.mongodb.com/guides/server/import/</t>
+  </si>
+  <si>
+    <t>https://kb.objectrocket.com/mongo-db/how-to-import-a-csv-into-mongodb-327</t>
+  </si>
+  <si>
+    <t>How to import a CSV into MongoDB</t>
+  </si>
+  <si>
+    <t>Import data into Mongo official docs</t>
+  </si>
+  <si>
+    <t>TypeScript crash course</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +271,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -219,10 +297,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -266,8 +345,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -776,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9956F9-8D97-449D-ACB5-C214B797C256}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,16 +878,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>44292</v>
+        <v>44293</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -979,7 +1065,265 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828DC6C4-C1E1-48A2-AC4B-AE446146FFE9}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>44294</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1" xr:uid="{C6A95AFC-4B9C-43FF-AE00-87AD0CEED2D9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010066F314D42E70FB4F962E325C4CCF27EF" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86d0c5eb7680b22b55b1b53511c5c4fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="282a6439-55bf-4e0c-8e7b-3c6254bfab40" xmlns:ns3="2154648b-c288-4c61-a630-f86fa10bab94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7837bdda419d93c8125662830abb78fc" ns2:_="" ns3:_="">
     <xsd:import namespace="282a6439-55bf-4e0c-8e7b-3c6254bfab40"/>
@@ -1190,22 +1534,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554B47C3-3F6D-4003-832E-345C67DC1627}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCCBE95-A568-4A35-B9D0-DC8154115CD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C442173E-CB06-4477-91A5-257B519F1064}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1222,21 +1568,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCCBE95-A568-4A35-B9D0-DC8154115CD7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554B47C3-3F6D-4003-832E-345C67DC1627}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
trying to import csv file
</commit_message>
<xml_diff>
--- a/Minutes/April Minutes.xlsx
+++ b/Minutes/April Minutes.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessw\Documents\Group Project\desk23\Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE8D51A-955E-4082-9F13-CE3B15D561A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B5AF54-2E9E-42DC-90DD-804943463070}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="300" windowWidth="14775" windowHeight="15300" activeTab="2" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
+    <workbookView xWindow="1110" yWindow="300" windowWidth="14775" windowHeight="15300" activeTab="3" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
   </bookViews>
   <sheets>
     <sheet name="0604" sheetId="1" r:id="rId1"/>
     <sheet name="0704" sheetId="2" r:id="rId2"/>
     <sheet name="0804" sheetId="3" r:id="rId3"/>
+    <sheet name="1204" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
   <si>
     <t>Date:</t>
   </si>
@@ -213,6 +214,18 @@
   </si>
   <si>
     <t>TypeScript crash course</t>
+  </si>
+  <si>
+    <t>Working on it - encountered problems</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>Find out how to import data into mongo outside of Docker</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828DC6C4-C1E1-48A2-AC4B-AE446146FFE9}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,22 +1321,196 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEAB8C1-8FD2-4E26-A84D-63272D5F4138}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>44294</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010066F314D42E70FB4F962E325C4CCF27EF" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86d0c5eb7680b22b55b1b53511c5c4fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="282a6439-55bf-4e0c-8e7b-3c6254bfab40" xmlns:ns3="2154648b-c288-4c61-a630-f86fa10bab94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7837bdda419d93c8125662830abb78fc" ns2:_="" ns3:_="">
     <xsd:import namespace="282a6439-55bf-4e0c-8e7b-3c6254bfab40"/>
@@ -1534,24 +1721,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554B47C3-3F6D-4003-832E-345C67DC1627}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCCBE95-A568-4A35-B9D0-DC8154115CD7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C442173E-CB06-4477-91A5-257B519F1064}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1568,4 +1753,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCCBE95-A568-4A35-B9D0-DC8154115CD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554B47C3-3F6D-4003-832E-345C67DC1627}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated minutes, altered query functions to return data
</commit_message>
<xml_diff>
--- a/Minutes/April Minutes.xlsx
+++ b/Minutes/April Minutes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessw\Documents\Group Project\desk23\Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D2ADFE-16D1-4F05-8514-43C997605A97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04F4C9B-21E8-4FA7-963E-A7C719C6981A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
   </bookViews>
   <sheets>
     <sheet name="0604" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="1204" sheetId="4" r:id="rId4"/>
     <sheet name="1604" sheetId="5" r:id="rId5"/>
     <sheet name="1904" sheetId="6" r:id="rId6"/>
+    <sheet name="2204" sheetId="7" r:id="rId7"/>
+    <sheet name="2304" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="103">
   <si>
     <t>Date:</t>
   </si>
@@ -303,6 +305,51 @@
   </si>
   <si>
     <t>Design targets: start writing documentation initial sketches</t>
+  </si>
+  <si>
+    <t>Completed - should be ok as is</t>
+  </si>
+  <si>
+    <t>Review with Marceli - all on track in his opinion</t>
+  </si>
+  <si>
+    <t>Working on it - completed GET functions, need to test (problems with Docker)</t>
+  </si>
+  <si>
+    <t>Working on it - working on tool tips and movements (problems with integrating with Angular)</t>
+  </si>
+  <si>
+    <t>Progress made, problems with linking d3 and Angular</t>
+  </si>
+  <si>
+    <t>Progress made, Wenda having problems with Docker making it hard to test - Jess has built some database query functions, need to alter to return value instead of just printing)</t>
+  </si>
+  <si>
+    <t>Completed (needs testing)</t>
+  </si>
+  <si>
+    <t>Progress made - created "working plan" document for everyone to work on their sections in</t>
+  </si>
+  <si>
+    <t>Next week</t>
+  </si>
+  <si>
+    <t>Emily to lead</t>
+  </si>
+  <si>
+    <t>Front end targets: display data on website and make it look nice, then add slider in later</t>
+  </si>
+  <si>
+    <t>Front end targets: connecting front end and back end, looking at timeline, tool tips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design targets: start testing, help with other tasks, learn a bit of HTML and CSS </t>
+  </si>
+  <si>
+    <t>Back end targets: connecting front and back end, think about slider</t>
+  </si>
+  <si>
+    <t>Back end targets: check database volumes are correct on each branch, get functions returning data instead of just printing to the console</t>
   </si>
 </sst>
 </file>
@@ -762,16 +809,16 @@
       <selection sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -780,7 +827,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -789,19 +836,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -810,29 +857,29 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="9"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="13"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
@@ -843,7 +890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
@@ -852,7 +899,7 @@
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
@@ -861,7 +908,7 @@
       </c>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -870,19 +917,19 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>18</v>
       </c>
@@ -892,7 +939,7 @@
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>20</v>
       </c>
@@ -902,19 +949,19 @@
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
@@ -923,23 +970,23 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="8"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
       <c r="B25" s="11"/>
     </row>
@@ -956,14 +1003,14 @@
       <selection sqref="A1:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -972,7 +1019,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -981,19 +1028,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1002,7 +1049,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
@@ -1011,7 +1058,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1020,7 +1067,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
@@ -1029,19 +1076,19 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
@@ -1052,7 +1099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>27</v>
       </c>
@@ -1063,7 +1110,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>29</v>
       </c>
@@ -1074,7 +1121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
@@ -1085,7 +1132,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>35</v>
       </c>
@@ -1096,7 +1143,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>33</v>
       </c>
@@ -1107,41 +1154,41 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>10</v>
       </c>
@@ -1163,14 +1210,14 @@
       <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1179,7 +1226,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1188,19 +1235,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1209,7 +1256,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>39</v>
       </c>
@@ -1218,7 +1265,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1227,7 +1274,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>25</v>
       </c>
@@ -1236,7 +1283,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
@@ -1245,7 +1292,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
@@ -1254,19 +1301,19 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
@@ -1277,7 +1324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>44</v>
       </c>
@@ -1288,7 +1335,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>47</v>
       </c>
@@ -1299,7 +1346,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>49</v>
       </c>
@@ -1310,7 +1357,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>51</v>
       </c>
@@ -1321,43 +1368,43 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>10</v>
       </c>
@@ -1366,7 +1413,7 @@
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>58</v>
       </c>
@@ -1374,7 +1421,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>57</v>
       </c>
@@ -1382,7 +1429,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>56</v>
       </c>
@@ -1406,14 +1453,14 @@
       <selection sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1469,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1431,19 +1478,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1452,7 +1499,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>39</v>
       </c>
@@ -1461,7 +1508,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>44</v>
       </c>
@@ -1470,7 +1517,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
@@ -1479,7 +1526,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>47</v>
       </c>
@@ -1488,7 +1535,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>43</v>
       </c>
@@ -1497,7 +1544,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
@@ -1506,7 +1553,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>51</v>
       </c>
@@ -1515,19 +1562,19 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
@@ -1538,7 +1585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>62</v>
       </c>
@@ -1549,31 +1596,31 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>10</v>
       </c>
@@ -1595,14 +1642,14 @@
       <selection sqref="A1:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1611,7 +1658,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1620,19 +1667,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1641,7 +1688,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>39</v>
       </c>
@@ -1650,7 +1697,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>44</v>
       </c>
@@ -1659,7 +1706,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
@@ -1668,7 +1715,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>47</v>
       </c>
@@ -1677,7 +1724,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>43</v>
       </c>
@@ -1686,7 +1733,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
@@ -1695,7 +1742,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>51</v>
       </c>
@@ -1704,7 +1751,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>62</v>
       </c>
@@ -1713,19 +1760,19 @@
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>3</v>
       </c>
@@ -1736,7 +1783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>64</v>
       </c>
@@ -1747,7 +1794,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>66</v>
       </c>
@@ -1758,7 +1805,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>68</v>
       </c>
@@ -1769,38 +1816,38 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>10</v>
       </c>
@@ -1809,7 +1856,7 @@
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>70</v>
       </c>
@@ -1827,18 +1874,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B981483-65BB-4036-A848-DE7E2829A5F8}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E22:E23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1847,7 +1894,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1856,19 +1903,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1877,7 +1924,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
@@ -1886,7 +1933,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>43</v>
       </c>
@@ -1895,7 +1942,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>41</v>
       </c>
@@ -1904,7 +1951,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>51</v>
       </c>
@@ -1913,7 +1960,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>64</v>
       </c>
@@ -1922,7 +1969,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>66</v>
       </c>
@@ -1931,12 +1978,12 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>68</v>
       </c>
@@ -1947,19 +1994,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>3</v>
       </c>
@@ -1970,7 +2017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>78</v>
       </c>
@@ -1981,7 +2028,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>80</v>
       </c>
@@ -1992,7 +2039,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>81</v>
       </c>
@@ -2003,7 +2050,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>82</v>
       </c>
@@ -2014,7 +2061,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>85</v>
       </c>
@@ -2025,7 +2072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>87</v>
       </c>
@@ -2036,38 +2083,38 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>77</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
@@ -2076,13 +2123,439 @@
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>71</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB477F1-787E-4BBF-93F6-992136DB352E}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>44308</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86882D91-3DD8-4F60-8ECB-6AEDC4F6A075}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>44309</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2090,21 +2563,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010066F314D42E70FB4F962E325C4CCF27EF" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86d0c5eb7680b22b55b1b53511c5c4fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="282a6439-55bf-4e0c-8e7b-3c6254bfab40" xmlns:ns3="2154648b-c288-4c61-a630-f86fa10bab94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7837bdda419d93c8125662830abb78fc" ns2:_="" ns3:_="">
     <xsd:import namespace="282a6439-55bf-4e0c-8e7b-3c6254bfab40"/>
@@ -2315,24 +2773,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554B47C3-3F6D-4003-832E-345C67DC1627}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCCBE95-A568-4A35-B9D0-DC8154115CD7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C442173E-CB06-4477-91A5-257B519F1064}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2349,4 +2805,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCCBE95-A568-4A35-B9D0-DC8154115CD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554B47C3-3F6D-4003-832E-345C67DC1627}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
trying to repopulate database with join table
</commit_message>
<xml_diff>
--- a/Minutes/April Minutes.xlsx
+++ b/Minutes/April Minutes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessw\Documents\Group Project\desk23\Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04F4C9B-21E8-4FA7-963E-A7C719C6981A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA4CF00-32E6-4F7B-83DF-C8547F7CF273}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="8" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
   </bookViews>
   <sheets>
     <sheet name="0604" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="1904" sheetId="6" r:id="rId6"/>
     <sheet name="2204" sheetId="7" r:id="rId7"/>
     <sheet name="2304" sheetId="8" r:id="rId8"/>
+    <sheet name="2604" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="113">
   <si>
     <t>Date:</t>
   </si>
@@ -350,6 +351,36 @@
   </si>
   <si>
     <t>Back end targets: check database volumes are correct on each branch, get functions returning data instead of just printing to the console</t>
+  </si>
+  <si>
+    <t>Working on it - need to integrate with front end</t>
+  </si>
+  <si>
+    <t>Working on it - difficult bugs to fix encountered linking d3 and Angular</t>
+  </si>
+  <si>
+    <t>Start writing documentation</t>
+  </si>
+  <si>
+    <t>Routing: perhaps have a separate page for book animation</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Combine data and coordinate collections</t>
+  </si>
+  <si>
+    <t>Start testing</t>
+  </si>
+  <si>
+    <t>Document framework/methodology for feedback</t>
+  </si>
+  <si>
+    <t>Wenda/Stanni/Hamza</t>
+  </si>
+  <si>
+    <t>Test Wenda's functions and let him know if there are errors</t>
   </si>
 </sst>
 </file>
@@ -809,16 +840,16 @@
       <selection sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,7 +858,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -836,19 +867,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -857,29 +888,29 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="9"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="13"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
@@ -890,7 +921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
@@ -899,7 +930,7 @@
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
@@ -908,7 +939,7 @@
       </c>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -917,19 +948,19 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>18</v>
       </c>
@@ -939,7 +970,7 @@
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>20</v>
       </c>
@@ -949,19 +980,19 @@
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
@@ -970,23 +1001,23 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="8"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="11"/>
     </row>
@@ -1003,14 +1034,14 @@
       <selection sqref="A1:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1050,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1028,19 +1059,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1049,7 +1080,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
@@ -1058,7 +1089,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1067,7 +1098,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
@@ -1076,19 +1107,19 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
@@ -1099,7 +1130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>27</v>
       </c>
@@ -1110,7 +1141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>29</v>
       </c>
@@ -1121,7 +1152,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
@@ -1132,7 +1163,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>35</v>
       </c>
@@ -1143,7 +1174,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>33</v>
       </c>
@@ -1154,41 +1185,41 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>10</v>
       </c>
@@ -1210,14 +1241,14 @@
       <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1257,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1235,19 +1266,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1256,7 +1287,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>39</v>
       </c>
@@ -1265,7 +1296,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -1274,7 +1305,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>25</v>
       </c>
@@ -1283,7 +1314,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
@@ -1292,7 +1323,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
@@ -1301,19 +1332,19 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
@@ -1324,7 +1355,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>44</v>
       </c>
@@ -1335,7 +1366,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>47</v>
       </c>
@@ -1346,7 +1377,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>49</v>
       </c>
@@ -1357,7 +1388,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>51</v>
       </c>
@@ -1368,43 +1399,43 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>10</v>
       </c>
@@ -1413,7 +1444,7 @@
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>58</v>
       </c>
@@ -1421,7 +1452,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>57</v>
       </c>
@@ -1429,7 +1460,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>56</v>
       </c>
@@ -1453,14 +1484,14 @@
       <selection sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1500,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1478,19 +1509,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1499,7 +1530,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>39</v>
       </c>
@@ -1508,7 +1539,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>44</v>
       </c>
@@ -1517,7 +1548,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
@@ -1526,7 +1557,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>47</v>
       </c>
@@ -1535,7 +1566,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>43</v>
       </c>
@@ -1544,7 +1575,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
@@ -1553,7 +1584,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>51</v>
       </c>
@@ -1562,19 +1593,19 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
@@ -1585,7 +1616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>62</v>
       </c>
@@ -1596,31 +1627,31 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>10</v>
       </c>
@@ -1642,14 +1673,14 @@
       <selection sqref="A1:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1689,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1667,19 +1698,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1688,7 +1719,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>39</v>
       </c>
@@ -1697,7 +1728,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>44</v>
       </c>
@@ -1706,7 +1737,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>49</v>
       </c>
@@ -1715,7 +1746,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>47</v>
       </c>
@@ -1724,7 +1755,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>43</v>
       </c>
@@ -1733,7 +1764,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
@@ -1742,7 +1773,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>51</v>
       </c>
@@ -1751,7 +1782,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>62</v>
       </c>
@@ -1760,19 +1791,19 @@
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>3</v>
       </c>
@@ -1783,7 +1814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>64</v>
       </c>
@@ -1794,7 +1825,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>66</v>
       </c>
@@ -1805,7 +1836,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>68</v>
       </c>
@@ -1816,38 +1847,38 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>10</v>
       </c>
@@ -1856,7 +1887,7 @@
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>70</v>
       </c>
@@ -1878,14 +1909,14 @@
       <selection activeCell="A17" sqref="A17:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1894,7 +1925,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -1903,19 +1934,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1924,7 +1955,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
@@ -1933,7 +1964,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>43</v>
       </c>
@@ -1942,7 +1973,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>41</v>
       </c>
@@ -1951,7 +1982,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>51</v>
       </c>
@@ -1960,7 +1991,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>64</v>
       </c>
@@ -1969,7 +2000,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>66</v>
       </c>
@@ -1978,12 +2009,12 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>68</v>
       </c>
@@ -1994,19 +2025,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>3</v>
       </c>
@@ -2017,7 +2048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>78</v>
       </c>
@@ -2028,7 +2059,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>80</v>
       </c>
@@ -2039,7 +2070,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>81</v>
       </c>
@@ -2050,7 +2081,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>82</v>
       </c>
@@ -2061,7 +2092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>85</v>
       </c>
@@ -2072,7 +2103,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>87</v>
       </c>
@@ -2083,38 +2114,38 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>77</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
@@ -2123,7 +2154,7 @@
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>70</v>
       </c>
@@ -2141,16 +2172,16 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D13"/>
+      <selection activeCell="A16" activeCellId="1" sqref="A15 A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2159,7 +2190,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -2168,19 +2199,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2189,7 +2220,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
@@ -2198,7 +2229,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>41</v>
       </c>
@@ -2207,7 +2238,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>64</v>
       </c>
@@ -2216,7 +2247,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>66</v>
       </c>
@@ -2225,7 +2256,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>68</v>
       </c>
@@ -2234,19 +2265,19 @@
       </c>
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
@@ -2257,38 +2288,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>89</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
@@ -2297,7 +2328,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="15"/>
     </row>
@@ -2310,18 +2341,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86882D91-3DD8-4F60-8ECB-6AEDC4F6A075}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection sqref="A1:C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2330,7 +2361,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -2339,19 +2370,19 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -2360,7 +2391,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>43</v>
       </c>
@@ -2369,7 +2400,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>41</v>
       </c>
@@ -2378,7 +2409,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>64</v>
       </c>
@@ -2387,7 +2418,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>66</v>
       </c>
@@ -2396,7 +2427,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>68</v>
       </c>
@@ -2405,7 +2436,7 @@
       </c>
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>78</v>
       </c>
@@ -2414,7 +2445,7 @@
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>80</v>
       </c>
@@ -2423,7 +2454,7 @@
       </c>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>81</v>
       </c>
@@ -2432,7 +2463,7 @@
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>82</v>
       </c>
@@ -2441,7 +2472,7 @@
       </c>
       <c r="C14" s="12"/>
     </row>
-    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>85</v>
       </c>
@@ -2450,7 +2481,7 @@
       </c>
       <c r="C15" s="12"/>
     </row>
-    <row r="16" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>87</v>
       </c>
@@ -2459,14 +2490,14 @@
       </c>
       <c r="C16" s="12"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>3</v>
       </c>
@@ -2477,7 +2508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>98</v>
       </c>
@@ -2488,7 +2519,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>99</v>
       </c>
@@ -2499,7 +2530,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>101</v>
       </c>
@@ -2510,7 +2541,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>102</v>
       </c>
@@ -2521,7 +2552,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>100</v>
       </c>
@@ -2532,19 +2563,19 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>10</v>
       </c>
@@ -2553,9 +2584,227 @@
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E825ACE-8862-46A9-9483-F40D37A219F1}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>44312</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated minutes, working on docker-compose errors
</commit_message>
<xml_diff>
--- a/Minutes/April Minutes.xlsx
+++ b/Minutes/April Minutes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessw\Documents\Group Project\desk23\Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA4CF00-32E6-4F7B-83DF-C8547F7CF273}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED63309-6C4C-409F-AB95-079AED12D79C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="8" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{593D935D-DF05-41ED-B4AC-13EBFE7AA417}"/>
   </bookViews>
   <sheets>
     <sheet name="0604" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="2204" sheetId="7" r:id="rId7"/>
     <sheet name="2304" sheetId="8" r:id="rId8"/>
     <sheet name="2604" sheetId="9" r:id="rId9"/>
+    <sheet name="2904" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="124">
   <si>
     <t>Date:</t>
   </si>
@@ -381,6 +382,39 @@
   </si>
   <si>
     <t>Test Wenda's functions and let him know if there are errors</t>
+  </si>
+  <si>
+    <t>Working on it - connected d3 with Angular</t>
+  </si>
+  <si>
+    <t>Ongoing (lower priority)</t>
+  </si>
+  <si>
+    <t>Framework written</t>
+  </si>
+  <si>
+    <t>Meet tomorrow to connect front and back end</t>
+  </si>
+  <si>
+    <t>Jess, Hamza, Wenda</t>
+  </si>
+  <si>
+    <t>Tomorrow (30th)</t>
+  </si>
+  <si>
+    <t>Final evaulation: have a new group, similar but more formal procedure</t>
+  </si>
+  <si>
+    <t>End of next week</t>
+  </si>
+  <si>
+    <t>Create affinity diagramming</t>
+  </si>
+  <si>
+    <t>Hamza/Emily/Jess</t>
+  </si>
+  <si>
+    <t>Focus group is actually more of a codesign group - user driven process</t>
   </si>
 </sst>
 </file>
@@ -1026,6 +1060,246 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0998825-A709-416D-BA1D-55E340CA4BC9}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>44315</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9956F9-8D97-449D-ACB5-C214B797C256}">
   <dimension ref="A1:C23"/>
@@ -2597,8 +2871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E825ACE-8862-46A9-9483-F40D37A219F1}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2812,6 +3086,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010066F314D42E70FB4F962E325C4CCF27EF" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86d0c5eb7680b22b55b1b53511c5c4fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="282a6439-55bf-4e0c-8e7b-3c6254bfab40" xmlns:ns3="2154648b-c288-4c61-a630-f86fa10bab94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7837bdda419d93c8125662830abb78fc" ns2:_="" ns3:_="">
     <xsd:import namespace="282a6439-55bf-4e0c-8e7b-3c6254bfab40"/>
@@ -3022,22 +3311,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554B47C3-3F6D-4003-832E-345C67DC1627}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCCBE95-A568-4A35-B9D0-DC8154115CD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C442173E-CB06-4477-91A5-257B519F1064}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3054,21 +3345,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCCBE95-A568-4A35-B9D0-DC8154115CD7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554B47C3-3F6D-4003-832E-345C67DC1627}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>